<commit_message>
Diverse Fehlerbehebungen, NAWA-MV-Einlesefunktionen, S_Chron-Mischtox, Details in Plots
</commit_message>
<xml_diff>
--- a/inst/extdata/Dat_Qual_kriterien.xlsx
+++ b/inst/extdata/Dat_Qual_kriterien.xlsx
@@ -29679,18 +29679,42 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BC84EED32EDA7740B91C79AC0B47256F" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f5219caf6006ef374036e70768e8bb53">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d5e11d0132dc5bb78ad0fb0e89938ac">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BC84EED32EDA7740B91C79AC0B47256F" ma:contentTypeVersion="3" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8d32669e96da46b38e440b11a40f6976">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7aa04b60-c9b6-4cc5-a80a-c839ead70f79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f2e8f8cc9c7b73f991aafde62806cbc" ns2:_="">
+    <xsd:import namespace="7aa04b60-c9b6-4cc5-a80a-c839ead70f79"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
-              <xsd:all/>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
             </xsd:complexType>
           </xsd:element>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7aa04b60-c9b6-4cc5-a80a-c839ead70f79" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -29808,13 +29832,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1651452F-0002-454C-8E1F-002D28DDDE27}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A5D968A-6D5B-4D5E-9F80-4755968D3B26}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA9144EA-35D9-4D8C-B170-23B26AFC1398}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E2DFB2-0546-4C7C-8BF1-54834ED93B54}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E94BA40-8903-414F-9DBE-F21D15913ED6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60FBE44C-3D48-49C2-86AB-551F0C6B5714}"/>
 </file>
</xml_diff>